<commit_message>
add shipper menu /myinventorycontrol, state3>1, remove all at cart
</commit_message>
<xml_diff>
--- a/src/main/webapp/resources/xls/partsdata.xlsx
+++ b/src/main/webapp/resources/xls/partsdata.xlsx
@@ -66,7 +66,7 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>신규 파츠 등록용 시트</t>
+    <t>파츠정보 조회/등록</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -282,8 +282,36 @@
     <cellStyle name="쉼표 [0]" xfId="1" builtinId="6"/>
     <cellStyle name="표준" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <dxfs count="2">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFD7D7D7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
+  <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
+      <tableStyleElement type="wholeTable" dxfId="1"/>
+      <tableStyleElement type="headerRow" dxfId="0"/>
+    </tableStyle>
+  </tableStyles>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -581,9 +609,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5"/>
   <cols>

</xml_diff>

<commit_message>
add MSLLevel in tb_part, add /logview
</commit_message>
<xml_diff>
--- a/src/main/webapp/resources/xls/partsdata.xlsx
+++ b/src/main/webapp/resources/xls/partsdata.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>LGIT P/N</t>
   </si>
@@ -67,6 +67,10 @@
   </si>
   <si>
     <t>파츠정보 조회/등록</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>MSL Level</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -206,21 +210,6 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
         <color auto="1"/>
       </left>
       <right style="thin">
@@ -234,6 +223,19 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
@@ -250,16 +252,10 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="8" fillId="0" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="8" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1">
@@ -268,14 +264,20 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -609,17 +611,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H8" sqref="H8"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5"/>
   <cols>
     <col min="1" max="1" width="13" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12.375" customWidth="1"/>
     <col min="3" max="7" width="9.875" customWidth="1"/>
+    <col min="8" max="8" width="12.5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="18.75">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="4" t="s">
         <v>13</v>
       </c>
       <c r="B1" s="1"/>
@@ -633,56 +638,59 @@
     <row r="3" spans="1:8">
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
-      <c r="F3" s="7" t="s">
+      <c r="G3" s="5" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:8">
-      <c r="A4" s="8" t="s">
+      <c r="A4" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="8" t="s">
+      <c r="B4" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="8" t="s">
+      <c r="C4" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="D4" s="9" t="s">
+      <c r="D4" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="E4" s="10" t="s">
+      <c r="E4" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="F4" s="10" t="s">
+      <c r="F4" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="G4" s="10" t="s">
+      <c r="G4" s="8" t="s">
         <v>9</v>
+      </c>
+      <c r="H4" s="8" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="5" spans="1:8">
-      <c r="A5" s="3" t="s">
+      <c r="A5" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="B5" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="C5" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D5" s="4" t="s">
+      <c r="D5" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="E5" s="5">
+      <c r="E5" s="3">
         <v>4000</v>
       </c>
-      <c r="F5" s="4" t="s">
+      <c r="F5" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="G5" s="2">
+      <c r="G5" s="10">
         <v>0.123</v>
       </c>
-      <c r="H5" s="2"/>
+      <c r="H5" s="10"/>
     </row>
     <row r="6" spans="1:8">
       <c r="A6" s="1"/>

</xml_diff>